<commit_message>
On branch main Your branch is up to date with 'deepaxon/main'.
Changes to be committed:
	modified:   Charles Data.xlsx
	modified:   __pycache__/morphometrics.cpython-38.pyc
	modified:   charles_daseg_morph.ipynb
	new file:   control_stats.ipynb
	modified:   morphometrics.py
	renamed:    morphometrics.ipynb -> notebooks/morphometrics.ipynb
	renamed:    new_morphometrics.ipynb -> notebooks/new_morphometrics.ipynb
	modified:   prelim_analysis.ipynb
	deleted:    ~$Charles Data.xlsx
</commit_message>
<xml_diff>
--- a/Charles Data.xlsx
+++ b/Charles Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Isaacs Lab\DeepAxon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D597EFED-376B-4063-990A-FBA9DAC3E25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED007EE-766A-4C32-BAEB-6D5B6E060F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="27072" windowHeight="16272" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animal Tracking" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Full Data (Per Image)" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Full Data (Per Image)'!$A$1:$K$781</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Full Data (Per Image)'!$A$1:$K$895</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Full Data (Per Nerve)'!$A$1:$K$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5772" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6114" uniqueCount="481">
   <si>
     <t>Batch</t>
   </si>
@@ -1481,7 +1481,10 @@
     <t>da_avg</t>
   </si>
   <si>
-    <t>da_full</t>
+    <t>da_full_major</t>
+  </si>
+  <si>
+    <t>da_full_avg</t>
   </si>
 </sst>
 </file>
@@ -12856,11 +12859,11 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K838"/>
+  <dimension ref="A1:K895"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A803" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I815" sqref="I815"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A326" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L401" sqref="L401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -39736,7 +39739,7 @@
         <v>2.9997286020813898</v>
       </c>
     </row>
-    <row r="782" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="782" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A782" s="1" t="s">
         <v>34</v>
       </c>
@@ -39750,7 +39753,7 @@
         <v>0</v>
       </c>
       <c r="E782" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F782" s="1" t="s">
         <v>156</v>
@@ -39771,7 +39774,7 @@
         <v>2.1871126844311002</v>
       </c>
     </row>
-    <row r="783" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="783" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A783" s="1" t="s">
         <v>34</v>
       </c>
@@ -39785,7 +39788,7 @@
         <v>0</v>
       </c>
       <c r="E783" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F783" s="1" t="s">
         <v>159</v>
@@ -39806,7 +39809,7 @@
         <v>2.2489149016944801</v>
       </c>
     </row>
-    <row r="784" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="784" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A784" s="1" t="s">
         <v>34</v>
       </c>
@@ -39820,7 +39823,7 @@
         <v>0</v>
       </c>
       <c r="E784" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F784" s="1" t="s">
         <v>162</v>
@@ -39841,7 +39844,7 @@
         <v>2.3754395392555199</v>
       </c>
     </row>
-    <row r="785" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="785" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A785" s="1" t="s">
         <v>34</v>
       </c>
@@ -39855,7 +39858,7 @@
         <v>0</v>
       </c>
       <c r="E785" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F785" s="1" t="s">
         <v>165</v>
@@ -39876,7 +39879,7 @@
         <v>2.4696956949100399</v>
       </c>
     </row>
-    <row r="786" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="786" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A786" s="1" t="s">
         <v>34</v>
       </c>
@@ -39890,7 +39893,7 @@
         <v>0</v>
       </c>
       <c r="E786" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F786" s="1" t="s">
         <v>168</v>
@@ -39911,7 +39914,7 @@
         <v>2.1285933043126</v>
       </c>
     </row>
-    <row r="787" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="787" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A787" s="1" t="s">
         <v>34</v>
       </c>
@@ -39925,7 +39928,7 @@
         <v>0</v>
       </c>
       <c r="E787" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F787" s="1" t="s">
         <v>171</v>
@@ -39946,7 +39949,7 @@
         <v>2.3819014339461502</v>
       </c>
     </row>
-    <row r="788" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="788" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A788" s="1" t="s">
         <v>34</v>
       </c>
@@ -39960,7 +39963,7 @@
         <v>0</v>
       </c>
       <c r="E788" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F788" s="1" t="s">
         <v>198</v>
@@ -39981,7 +39984,7 @@
         <v>3.1840708345884399</v>
       </c>
     </row>
-    <row r="789" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="789" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A789" s="1" t="s">
         <v>38</v>
       </c>
@@ -39995,7 +39998,7 @@
         <v>0</v>
       </c>
       <c r="E789" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F789" s="1" t="s">
         <v>156</v>
@@ -40016,7 +40019,7 @@
         <v>2.26306021984198</v>
       </c>
     </row>
-    <row r="790" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="790" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A790" s="1" t="s">
         <v>38</v>
       </c>
@@ -40030,7 +40033,7 @@
         <v>0</v>
       </c>
       <c r="E790" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F790" s="1" t="s">
         <v>159</v>
@@ -40051,7 +40054,7 @@
         <v>2.02733032669114</v>
       </c>
     </row>
-    <row r="791" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="791" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A791" s="1" t="s">
         <v>38</v>
       </c>
@@ -40065,7 +40068,7 @@
         <v>0</v>
       </c>
       <c r="E791" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F791" s="1" t="s">
         <v>162</v>
@@ -40086,7 +40089,7 @@
         <v>2.0876622097673798</v>
       </c>
     </row>
-    <row r="792" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="792" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A792" s="1" t="s">
         <v>38</v>
       </c>
@@ -40100,7 +40103,7 @@
         <v>0</v>
       </c>
       <c r="E792" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F792" s="1" t="s">
         <v>165</v>
@@ -40121,7 +40124,7 @@
         <v>2.0939660255274899</v>
       </c>
     </row>
-    <row r="793" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="793" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A793" s="1" t="s">
         <v>38</v>
       </c>
@@ -40135,7 +40138,7 @@
         <v>0</v>
       </c>
       <c r="E793" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F793" s="1" t="s">
         <v>168</v>
@@ -40156,7 +40159,7 @@
         <v>2.5549422859986901</v>
       </c>
     </row>
-    <row r="794" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="794" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A794" s="1" t="s">
         <v>38</v>
       </c>
@@ -40170,7 +40173,7 @@
         <v>0</v>
       </c>
       <c r="E794" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F794" s="1" t="s">
         <v>171</v>
@@ -40191,7 +40194,7 @@
         <v>3.5313988445294302</v>
       </c>
     </row>
-    <row r="795" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="795" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A795" s="1" t="s">
         <v>38</v>
       </c>
@@ -40205,7 +40208,7 @@
         <v>0</v>
       </c>
       <c r="E795" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F795" s="1" t="s">
         <v>198</v>
@@ -40226,7 +40229,7 @@
         <v>2.8320597984847899</v>
       </c>
     </row>
-    <row r="796" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="796" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A796" s="1" t="s">
         <v>38</v>
       </c>
@@ -40240,7 +40243,7 @@
         <v>0</v>
       </c>
       <c r="E796" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F796" s="1" t="s">
         <v>253</v>
@@ -40261,7 +40264,7 @@
         <v>2.2744060634990499</v>
       </c>
     </row>
-    <row r="797" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="797" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A797" s="1" t="s">
         <v>40</v>
       </c>
@@ -40275,7 +40278,7 @@
         <v>0</v>
       </c>
       <c r="E797" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F797" s="1" t="s">
         <v>156</v>
@@ -40296,7 +40299,7 @@
         <v>2.2025271835039399</v>
       </c>
     </row>
-    <row r="798" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="798" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A798" s="1" t="s">
         <v>40</v>
       </c>
@@ -40310,7 +40313,7 @@
         <v>0</v>
       </c>
       <c r="E798" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F798" s="1" t="s">
         <v>159</v>
@@ -40331,7 +40334,7 @@
         <v>2.8948496591852502</v>
       </c>
     </row>
-    <row r="799" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="799" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A799" s="1" t="s">
         <v>40</v>
       </c>
@@ -40345,7 +40348,7 @@
         <v>0</v>
       </c>
       <c r="E799" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F799" s="1" t="s">
         <v>162</v>
@@ -40366,7 +40369,7 @@
         <v>2.6313780238398299</v>
       </c>
     </row>
-    <row r="800" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="800" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A800" s="1" t="s">
         <v>40</v>
       </c>
@@ -40380,7 +40383,7 @@
         <v>0</v>
       </c>
       <c r="E800" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F800" s="1" t="s">
         <v>165</v>
@@ -40401,7 +40404,7 @@
         <v>1.87990203682955</v>
       </c>
     </row>
-    <row r="801" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="801" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A801" s="1" t="s">
         <v>40</v>
       </c>
@@ -40415,7 +40418,7 @@
         <v>0</v>
       </c>
       <c r="E801" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F801" s="1" t="s">
         <v>168</v>
@@ -40436,7 +40439,7 @@
         <v>1.9466712197286899</v>
       </c>
     </row>
-    <row r="802" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="802" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A802" s="1" t="s">
         <v>40</v>
       </c>
@@ -40450,7 +40453,7 @@
         <v>0</v>
       </c>
       <c r="E802" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F802" s="1" t="s">
         <v>171</v>
@@ -40471,7 +40474,7 @@
         <v>2.4300512793044402</v>
       </c>
     </row>
-    <row r="803" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="803" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A803" s="1" t="s">
         <v>40</v>
       </c>
@@ -40485,7 +40488,7 @@
         <v>0</v>
       </c>
       <c r="E803" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F803" s="1" t="s">
         <v>198</v>
@@ -40506,7 +40509,7 @@
         <v>2.1648555136088499</v>
       </c>
     </row>
-    <row r="804" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="804" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A804" s="1" t="s">
         <v>50</v>
       </c>
@@ -40520,7 +40523,7 @@
         <v>1</v>
       </c>
       <c r="E804" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F804" s="1" t="s">
         <v>156</v>
@@ -40541,7 +40544,7 @@
         <v>2.22611764946932</v>
       </c>
     </row>
-    <row r="805" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="805" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A805" s="1" t="s">
         <v>50</v>
       </c>
@@ -40555,7 +40558,7 @@
         <v>1</v>
       </c>
       <c r="E805" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F805" s="1" t="s">
         <v>159</v>
@@ -40576,7 +40579,7 @@
         <v>2.15631820831153</v>
       </c>
     </row>
-    <row r="806" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="806" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A806" s="1" t="s">
         <v>50</v>
       </c>
@@ -40590,7 +40593,7 @@
         <v>1</v>
       </c>
       <c r="E806" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F806" s="1" t="s">
         <v>162</v>
@@ -40611,7 +40614,7 @@
         <v>2.5516568945174698</v>
       </c>
     </row>
-    <row r="807" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="807" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A807" s="1" t="s">
         <v>50</v>
       </c>
@@ -40625,7 +40628,7 @@
         <v>1</v>
       </c>
       <c r="E807" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F807" s="1" t="s">
         <v>165</v>
@@ -40646,7 +40649,7 @@
         <v>3.1349491032690802</v>
       </c>
     </row>
-    <row r="808" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="808" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A808" s="1" t="s">
         <v>50</v>
       </c>
@@ -40660,7 +40663,7 @@
         <v>1</v>
       </c>
       <c r="E808" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F808" s="1" t="s">
         <v>168</v>
@@ -40681,7 +40684,7 @@
         <v>2.0666288489542701</v>
       </c>
     </row>
-    <row r="809" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="809" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A809" s="1" t="s">
         <v>50</v>
       </c>
@@ -40695,7 +40698,7 @@
         <v>1</v>
       </c>
       <c r="E809" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F809" s="1" t="s">
         <v>171</v>
@@ -40716,7 +40719,7 @@
         <v>2.2862643234423699</v>
       </c>
     </row>
-    <row r="810" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="810" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A810" s="1" t="s">
         <v>48</v>
       </c>
@@ -40730,7 +40733,7 @@
         <v>0</v>
       </c>
       <c r="E810" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F810" s="1" t="s">
         <v>156</v>
@@ -40751,7 +40754,7 @@
         <v>2.5578560079189998</v>
       </c>
     </row>
-    <row r="811" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="811" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A811" s="1" t="s">
         <v>48</v>
       </c>
@@ -40765,7 +40768,7 @@
         <v>0</v>
       </c>
       <c r="E811" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F811" s="1" t="s">
         <v>159</v>
@@ -40786,7 +40789,7 @@
         <v>2.5133334512616701</v>
       </c>
     </row>
-    <row r="812" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="812" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A812" s="1" t="s">
         <v>48</v>
       </c>
@@ -40800,7 +40803,7 @@
         <v>0</v>
       </c>
       <c r="E812" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F812" s="1" t="s">
         <v>162</v>
@@ -40821,7 +40824,7 @@
         <v>2.6440837279060698</v>
       </c>
     </row>
-    <row r="813" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="813" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A813" s="1" t="s">
         <v>48</v>
       </c>
@@ -40835,7 +40838,7 @@
         <v>0</v>
       </c>
       <c r="E813" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F813" s="1" t="s">
         <v>165</v>
@@ -40856,7 +40859,7 @@
         <v>2.6891531089466199</v>
       </c>
     </row>
-    <row r="814" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="814" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A814" s="1" t="s">
         <v>48</v>
       </c>
@@ -40870,7 +40873,7 @@
         <v>0</v>
       </c>
       <c r="E814" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F814" s="1" t="s">
         <v>168</v>
@@ -40891,7 +40894,7 @@
         <v>2.45174736431514</v>
       </c>
     </row>
-    <row r="815" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="815" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A815" s="1" t="s">
         <v>48</v>
       </c>
@@ -40905,7 +40908,7 @@
         <v>0</v>
       </c>
       <c r="E815" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F815" s="1" t="s">
         <v>171</v>
@@ -40926,7 +40929,7 @@
         <v>2.49324066510958</v>
       </c>
     </row>
-    <row r="816" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="816" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A816" s="1" t="s">
         <v>46</v>
       </c>
@@ -40940,7 +40943,7 @@
         <v>0</v>
       </c>
       <c r="E816" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F816" s="1" t="s">
         <v>156</v>
@@ -40961,7 +40964,7 @@
         <v>2.6430620430690199</v>
       </c>
     </row>
-    <row r="817" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="817" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A817" s="1" t="s">
         <v>46</v>
       </c>
@@ -40975,7 +40978,7 @@
         <v>0</v>
       </c>
       <c r="E817" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F817" s="1" t="s">
         <v>159</v>
@@ -40996,7 +40999,7 @@
         <v>2.2904460593600899</v>
       </c>
     </row>
-    <row r="818" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="818" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A818" s="1" t="s">
         <v>46</v>
       </c>
@@ -41010,7 +41013,7 @@
         <v>0</v>
       </c>
       <c r="E818" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F818" s="1" t="s">
         <v>162</v>
@@ -41031,7 +41034,7 @@
         <v>2.3928381782538</v>
       </c>
     </row>
-    <row r="819" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="819" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A819" s="1" t="s">
         <v>46</v>
       </c>
@@ -41045,7 +41048,7 @@
         <v>0</v>
       </c>
       <c r="E819" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F819" s="1" t="s">
         <v>165</v>
@@ -41066,7 +41069,7 @@
         <v>2.5059932537053902</v>
       </c>
     </row>
-    <row r="820" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="820" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A820" s="1" t="s">
         <v>46</v>
       </c>
@@ -41080,7 +41083,7 @@
         <v>0</v>
       </c>
       <c r="E820" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F820" s="1" t="s">
         <v>168</v>
@@ -41101,7 +41104,7 @@
         <v>2.8287053664520099</v>
       </c>
     </row>
-    <row r="821" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="821" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A821" s="1" t="s">
         <v>46</v>
       </c>
@@ -41115,7 +41118,7 @@
         <v>0</v>
       </c>
       <c r="E821" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F821" s="1" t="s">
         <v>171</v>
@@ -41136,7 +41139,7 @@
         <v>2.7956849329090701</v>
       </c>
     </row>
-    <row r="822" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="822" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A822" s="1" t="s">
         <v>46</v>
       </c>
@@ -41150,7 +41153,7 @@
         <v>0</v>
       </c>
       <c r="E822" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F822" s="1" t="s">
         <v>198</v>
@@ -41171,7 +41174,7 @@
         <v>2.3683307324464198</v>
       </c>
     </row>
-    <row r="823" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="823" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A823" s="1" t="s">
         <v>46</v>
       </c>
@@ -41185,7 +41188,7 @@
         <v>0</v>
       </c>
       <c r="E823" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F823" s="1" t="s">
         <v>253</v>
@@ -41206,7 +41209,7 @@
         <v>2.4336176517558599</v>
       </c>
     </row>
-    <row r="824" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="824" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A824" s="1" t="s">
         <v>42</v>
       </c>
@@ -41220,7 +41223,7 @@
         <v>0</v>
       </c>
       <c r="E824" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F824" s="1" t="s">
         <v>156</v>
@@ -41241,7 +41244,7 @@
         <v>2.2671671858465201</v>
       </c>
     </row>
-    <row r="825" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="825" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A825" s="1" t="s">
         <v>42</v>
       </c>
@@ -41255,7 +41258,7 @@
         <v>0</v>
       </c>
       <c r="E825" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F825" s="1" t="s">
         <v>159</v>
@@ -41276,7 +41279,7 @@
         <v>2.2997511500451102</v>
       </c>
     </row>
-    <row r="826" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="826" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A826" s="1" t="s">
         <v>42</v>
       </c>
@@ -41290,7 +41293,7 @@
         <v>0</v>
       </c>
       <c r="E826" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F826" s="1" t="s">
         <v>162</v>
@@ -41311,7 +41314,7 @@
         <v>2.2789893778684398</v>
       </c>
     </row>
-    <row r="827" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="827" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A827" s="1" t="s">
         <v>42</v>
       </c>
@@ -41325,7 +41328,7 @@
         <v>0</v>
       </c>
       <c r="E827" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F827" s="1" t="s">
         <v>165</v>
@@ -41346,7 +41349,7 @@
         <v>2.2363984113374999</v>
       </c>
     </row>
-    <row r="828" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="828" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A828" s="1" t="s">
         <v>42</v>
       </c>
@@ -41360,7 +41363,7 @@
         <v>0</v>
       </c>
       <c r="E828" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F828" s="1" t="s">
         <v>168</v>
@@ -41381,7 +41384,7 @@
         <v>2.3141419857022099</v>
       </c>
     </row>
-    <row r="829" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="829" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A829" s="1" t="s">
         <v>42</v>
       </c>
@@ -41395,7 +41398,7 @@
         <v>0</v>
       </c>
       <c r="E829" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F829" s="1" t="s">
         <v>171</v>
@@ -41416,7 +41419,7 @@
         <v>2.4215740345043</v>
       </c>
     </row>
-    <row r="830" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="830" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A830" s="1" t="s">
         <v>42</v>
       </c>
@@ -41430,7 +41433,7 @@
         <v>0</v>
       </c>
       <c r="E830" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F830" s="1" t="s">
         <v>198</v>
@@ -41451,7 +41454,7 @@
         <v>2.4847913078497701</v>
       </c>
     </row>
-    <row r="831" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="831" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A831" s="1" t="s">
         <v>44</v>
       </c>
@@ -41465,7 +41468,7 @@
         <v>0</v>
       </c>
       <c r="E831" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F831" s="1" t="s">
         <v>156</v>
@@ -41486,7 +41489,7 @@
         <v>2.5694420653777201</v>
       </c>
     </row>
-    <row r="832" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="832" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A832" s="1" t="s">
         <v>44</v>
       </c>
@@ -41500,7 +41503,7 @@
         <v>0</v>
       </c>
       <c r="E832" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F832" s="1" t="s">
         <v>159</v>
@@ -41521,7 +41524,7 @@
         <v>3.0684991729862898</v>
       </c>
     </row>
-    <row r="833" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="833" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A833" s="1" t="s">
         <v>44</v>
       </c>
@@ -41535,7 +41538,7 @@
         <v>0</v>
       </c>
       <c r="E833" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F833" s="1" t="s">
         <v>162</v>
@@ -41556,7 +41559,7 @@
         <v>2.83764991882189</v>
       </c>
     </row>
-    <row r="834" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="834" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A834" s="1" t="s">
         <v>44</v>
       </c>
@@ -41570,7 +41573,7 @@
         <v>0</v>
       </c>
       <c r="E834" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F834" s="1" t="s">
         <v>165</v>
@@ -41591,7 +41594,7 @@
         <v>2.3633231747002998</v>
       </c>
     </row>
-    <row r="835" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="835" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A835" s="1" t="s">
         <v>44</v>
       </c>
@@ -41605,7 +41608,7 @@
         <v>0</v>
       </c>
       <c r="E835" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F835" s="1" t="s">
         <v>168</v>
@@ -41626,7 +41629,7 @@
         <v>1.96225449432612</v>
       </c>
     </row>
-    <row r="836" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="836" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A836" s="1" t="s">
         <v>44</v>
       </c>
@@ -41640,7 +41643,7 @@
         <v>0</v>
       </c>
       <c r="E836" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F836" s="1" t="s">
         <v>171</v>
@@ -41661,7 +41664,7 @@
         <v>1.8877679434683901</v>
       </c>
     </row>
-    <row r="837" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A837" s="1" t="s">
         <v>44</v>
       </c>
@@ -41675,7 +41678,7 @@
         <v>0</v>
       </c>
       <c r="E837" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F837" s="1" t="s">
         <v>198</v>
@@ -41696,7 +41699,7 @@
         <v>3.13087261329474</v>
       </c>
     </row>
-    <row r="838" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="838" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A838" s="1" t="s">
         <v>44</v>
       </c>
@@ -41710,7 +41713,7 @@
         <v>0</v>
       </c>
       <c r="E838" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F838" s="1" t="s">
         <v>253</v>
@@ -41731,8 +41734,2003 @@
         <v>2.99184259864154</v>
       </c>
     </row>
+    <row r="839" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A839" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B839" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C839" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D839" s="1">
+        <v>0</v>
+      </c>
+      <c r="E839" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F839" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G839" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H839" s="1">
+        <v>64586</v>
+      </c>
+      <c r="I839">
+        <v>1099</v>
+      </c>
+      <c r="J839">
+        <v>0.55689538239181002</v>
+      </c>
+      <c r="K839">
+        <v>2.6264271155526102</v>
+      </c>
+    </row>
+    <row r="840" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A840" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B840" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C840" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D840" s="1">
+        <v>0</v>
+      </c>
+      <c r="E840" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F840" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G840" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H840" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I840">
+        <v>928</v>
+      </c>
+      <c r="J840">
+        <v>0.61423577223301995</v>
+      </c>
+      <c r="K840">
+        <v>2.7654375843799799</v>
+      </c>
+    </row>
+    <row r="841" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A841" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B841" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C841" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D841" s="1">
+        <v>0</v>
+      </c>
+      <c r="E841" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F841" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G841" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H841" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I841">
+        <v>819</v>
+      </c>
+      <c r="J841">
+        <v>0.60567452938557498</v>
+      </c>
+      <c r="K841">
+        <v>2.9929594752461699</v>
+      </c>
+    </row>
+    <row r="842" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A842" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B842" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C842" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D842" s="1">
+        <v>0</v>
+      </c>
+      <c r="E842" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F842" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G842" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H842" s="1">
+        <v>55757</v>
+      </c>
+      <c r="I842">
+        <v>693</v>
+      </c>
+      <c r="J842">
+        <v>0.58763397027563902</v>
+      </c>
+      <c r="K842">
+        <v>3.2332346061500301</v>
+      </c>
+    </row>
+    <row r="843" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A843" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B843" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C843" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D843" s="1">
+        <v>0</v>
+      </c>
+      <c r="E843" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F843" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G843" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H843" s="1">
+        <v>65164</v>
+      </c>
+      <c r="I843">
+        <v>1048</v>
+      </c>
+      <c r="J843">
+        <v>0.59077530899518704</v>
+      </c>
+      <c r="K843">
+        <v>2.6395400130634199</v>
+      </c>
+    </row>
+    <row r="844" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A844" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B844" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C844" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D844" s="1">
+        <v>0</v>
+      </c>
+      <c r="E844" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F844" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G844" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H844" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I844">
+        <v>915</v>
+      </c>
+      <c r="J844">
+        <v>0.60788094121900105</v>
+      </c>
+      <c r="K844">
+        <v>3.0965200274702598</v>
+      </c>
+    </row>
+    <row r="845" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A845" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B845" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C845" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D845" s="1">
+        <v>0</v>
+      </c>
+      <c r="E845" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F845" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G845" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H845" s="1">
+        <v>60903</v>
+      </c>
+      <c r="I845">
+        <v>581</v>
+      </c>
+      <c r="J845">
+        <v>0.66288579212547505</v>
+      </c>
+      <c r="K845">
+        <v>3.8714930088542299</v>
+      </c>
+    </row>
+    <row r="846" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A846" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B846" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C846" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D846" s="1">
+        <v>0</v>
+      </c>
+      <c r="E846" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F846" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G846" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="H846" s="10">
+        <v>64764</v>
+      </c>
+      <c r="I846">
+        <v>908</v>
+      </c>
+      <c r="J846">
+        <v>0.64588342172642799</v>
+      </c>
+      <c r="K846">
+        <v>2.8864902313058698</v>
+      </c>
+    </row>
+    <row r="847" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A847" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B847" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C847" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D847" s="1">
+        <v>0</v>
+      </c>
+      <c r="E847" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F847" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G847" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="H847" s="10">
+        <v>66063</v>
+      </c>
+      <c r="I847">
+        <v>1045</v>
+      </c>
+      <c r="J847">
+        <v>0.68161402692795603</v>
+      </c>
+      <c r="K847">
+        <v>2.8334675008130099</v>
+      </c>
+    </row>
+    <row r="848" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A848" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B848" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C848" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D848" s="1">
+        <v>0</v>
+      </c>
+      <c r="E848" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F848" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G848" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="H848" s="10">
+        <v>66063</v>
+      </c>
+      <c r="I848">
+        <v>894</v>
+      </c>
+      <c r="J848">
+        <v>0.69160171481074695</v>
+      </c>
+      <c r="K848">
+        <v>2.94992739273138</v>
+      </c>
+    </row>
+    <row r="849" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A849" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B849" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C849" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D849" s="1">
+        <v>0</v>
+      </c>
+      <c r="E849" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F849" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G849" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="H849" s="10">
+        <v>66063</v>
+      </c>
+      <c r="I849">
+        <v>889</v>
+      </c>
+      <c r="J849">
+        <v>0.69097660292065899</v>
+      </c>
+      <c r="K849">
+        <v>2.9197688416382799</v>
+      </c>
+    </row>
+    <row r="850" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A850" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B850" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C850" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D850" s="1">
+        <v>0</v>
+      </c>
+      <c r="E850" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F850" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G850" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="H850" s="10">
+        <v>66063</v>
+      </c>
+      <c r="I850">
+        <v>773</v>
+      </c>
+      <c r="J850">
+        <v>0.69448734454527095</v>
+      </c>
+      <c r="K850">
+        <v>3.3495449424653598</v>
+      </c>
+    </row>
+    <row r="851" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A851" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B851" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C851" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D851" s="1">
+        <v>0</v>
+      </c>
+      <c r="E851" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F851" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G851" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="H851" s="10">
+        <v>56203</v>
+      </c>
+      <c r="I851">
+        <v>477</v>
+      </c>
+      <c r="J851">
+        <v>0.65690836637231698</v>
+      </c>
+      <c r="K851">
+        <v>4.3471253792993503</v>
+      </c>
+    </row>
+    <row r="852" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A852" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B852" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C852" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D852" s="1">
+        <v>0</v>
+      </c>
+      <c r="E852" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F852" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G852" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="H852" s="10">
+        <v>63646</v>
+      </c>
+      <c r="I852">
+        <v>586</v>
+      </c>
+      <c r="J852">
+        <v>0.69525964891006797</v>
+      </c>
+      <c r="K852">
+        <v>3.60045368145714</v>
+      </c>
+    </row>
+    <row r="853" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A853" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B853" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C853" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D853" s="1">
+        <v>0</v>
+      </c>
+      <c r="E853" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F853" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G853" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="H853" s="10">
+        <v>46992</v>
+      </c>
+      <c r="I853">
+        <v>739</v>
+      </c>
+      <c r="J853">
+        <v>0.66992998578042495</v>
+      </c>
+      <c r="K853">
+        <v>2.9640873442690201</v>
+      </c>
+    </row>
+    <row r="854" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A854" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B854" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C854" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D854" s="1">
+        <v>0</v>
+      </c>
+      <c r="E854" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F854" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G854" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H854" s="1">
+        <v>64456</v>
+      </c>
+      <c r="I854">
+        <v>401</v>
+      </c>
+      <c r="J854">
+        <v>0.65138952689992302</v>
+      </c>
+      <c r="K854">
+        <v>3.4507641374495202</v>
+      </c>
+    </row>
+    <row r="855" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A855" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B855" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C855" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D855" s="1">
+        <v>0</v>
+      </c>
+      <c r="E855" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F855" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G855" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H855" s="1">
+        <v>53018</v>
+      </c>
+      <c r="I855">
+        <v>305</v>
+      </c>
+      <c r="J855">
+        <v>0.66342384138785804</v>
+      </c>
+      <c r="K855">
+        <v>3.2635636818482401</v>
+      </c>
+    </row>
+    <row r="856" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A856" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B856" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C856" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D856" s="1">
+        <v>0</v>
+      </c>
+      <c r="E856" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F856" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G856" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H856" s="1">
+        <v>56530</v>
+      </c>
+      <c r="I856">
+        <v>692</v>
+      </c>
+      <c r="J856">
+        <v>0.65227585619458806</v>
+      </c>
+      <c r="K856">
+        <v>2.37832760768435</v>
+      </c>
+    </row>
+    <row r="857" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A857" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B857" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C857" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D857" s="1">
+        <v>0</v>
+      </c>
+      <c r="E857" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F857" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G857" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H857" s="1">
+        <v>57119</v>
+      </c>
+      <c r="I857">
+        <v>694</v>
+      </c>
+      <c r="J857">
+        <v>0.644320209676567</v>
+      </c>
+      <c r="K857">
+        <v>2.4370722643803302</v>
+      </c>
+    </row>
+    <row r="858" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A858" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B858" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C858" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D858" s="1">
+        <v>0</v>
+      </c>
+      <c r="E858" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F858" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G858" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H858" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I858">
+        <v>595</v>
+      </c>
+      <c r="J858">
+        <v>0.63876130007724397</v>
+      </c>
+      <c r="K858">
+        <v>3.0386125085577498</v>
+      </c>
+    </row>
+    <row r="859" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A859" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B859" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C859" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D859" s="1">
+        <v>0</v>
+      </c>
+      <c r="E859" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F859" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G859" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H859" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I859">
+        <v>750</v>
+      </c>
+      <c r="J859">
+        <v>0.66368601492294599</v>
+      </c>
+      <c r="K859">
+        <v>2.8138337631630401</v>
+      </c>
+    </row>
+    <row r="860" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A860" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B860" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C860" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D860" s="1">
+        <v>0</v>
+      </c>
+      <c r="E860" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F860" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G860" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H860" s="1">
+        <v>55004</v>
+      </c>
+      <c r="I860">
+        <v>581</v>
+      </c>
+      <c r="J860">
+        <v>0.67399337064255305</v>
+      </c>
+      <c r="K860">
+        <v>2.7870866837719399</v>
+      </c>
+    </row>
+    <row r="861" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A861" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B861" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C861" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D861" s="1">
+        <v>1</v>
+      </c>
+      <c r="E861" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F861" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G861" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="H861" s="1">
+        <v>64309</v>
+      </c>
+      <c r="I861">
+        <v>977</v>
+      </c>
+      <c r="J861">
+        <v>0.59494971299545096</v>
+      </c>
+      <c r="K861">
+        <v>2.77959012500602</v>
+      </c>
+    </row>
+    <row r="862" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A862" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B862" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C862" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D862" s="1">
+        <v>1</v>
+      </c>
+      <c r="E862" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F862" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G862" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H862" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I862">
+        <v>803</v>
+      </c>
+      <c r="J862">
+        <v>0.63764261771534902</v>
+      </c>
+      <c r="K862">
+        <v>2.7513950338350002</v>
+      </c>
+    </row>
+    <row r="863" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A863" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B863" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C863" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D863" s="1">
+        <v>1</v>
+      </c>
+      <c r="E863" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F863" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G863" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H863" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I863">
+        <v>736</v>
+      </c>
+      <c r="J863">
+        <v>0.64669424233918904</v>
+      </c>
+      <c r="K863">
+        <v>3.1681589092403502</v>
+      </c>
+    </row>
+    <row r="864" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A864" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B864" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C864" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D864" s="1">
+        <v>1</v>
+      </c>
+      <c r="E864" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F864" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G864" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H864" s="1">
+        <v>54749</v>
+      </c>
+      <c r="I864">
+        <v>458</v>
+      </c>
+      <c r="J864">
+        <v>0.66691078034533402</v>
+      </c>
+      <c r="K864">
+        <v>3.7067280168738499</v>
+      </c>
+    </row>
+    <row r="865" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A865" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B865" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C865" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D865" s="1">
+        <v>1</v>
+      </c>
+      <c r="E865" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F865" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G865" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="H865" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I865">
+        <v>993</v>
+      </c>
+      <c r="J865">
+        <v>0.62300241037243298</v>
+      </c>
+      <c r="K865">
+        <v>2.7389881270043901</v>
+      </c>
+    </row>
+    <row r="866" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A866" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B866" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C866" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D866" s="1">
+        <v>1</v>
+      </c>
+      <c r="E866" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F866" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G866" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H866" s="1">
+        <v>45278</v>
+      </c>
+      <c r="I866">
+        <v>752</v>
+      </c>
+      <c r="J866">
+        <v>0.58521149980398401</v>
+      </c>
+      <c r="K866">
+        <v>2.8718209287667298</v>
+      </c>
+    </row>
+    <row r="867" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A867" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B867" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C867" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D867" s="1">
+        <v>0</v>
+      </c>
+      <c r="E867" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F867" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G867" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H867" s="1">
+        <v>65642</v>
+      </c>
+      <c r="I867">
+        <v>748</v>
+      </c>
+      <c r="J867">
+        <v>0.62846928659795698</v>
+      </c>
+      <c r="K867">
+        <v>3.0443126735486499</v>
+      </c>
+    </row>
+    <row r="868" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A868" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B868" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C868" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D868" s="1">
+        <v>0</v>
+      </c>
+      <c r="E868" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F868" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G868" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H868" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I868">
+        <v>744</v>
+      </c>
+      <c r="J868">
+        <v>0.67871766934077604</v>
+      </c>
+      <c r="K868">
+        <v>2.9923567532889801</v>
+      </c>
+    </row>
+    <row r="869" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A869" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B869" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C869" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D869" s="1">
+        <v>0</v>
+      </c>
+      <c r="E869" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F869" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G869" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H869" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I869">
+        <v>693</v>
+      </c>
+      <c r="J869">
+        <v>0.68344597405451901</v>
+      </c>
+      <c r="K869">
+        <v>3.2317098307382701</v>
+      </c>
+    </row>
+    <row r="870" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A870" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B870" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C870" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D870" s="1">
+        <v>0</v>
+      </c>
+      <c r="E870" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F870" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G870" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H870" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I870">
+        <v>676</v>
+      </c>
+      <c r="J870">
+        <v>0.66933471409470402</v>
+      </c>
+      <c r="K870">
+        <v>3.2437845320343999</v>
+      </c>
+    </row>
+    <row r="871" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A871" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B871" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C871" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D871" s="1">
+        <v>0</v>
+      </c>
+      <c r="E871" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F871" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G871" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H871" s="1">
+        <v>65520</v>
+      </c>
+      <c r="I871">
+        <v>883</v>
+      </c>
+      <c r="J871">
+        <v>0.66829627620922005</v>
+      </c>
+      <c r="K871">
+        <v>3.1005915443668202</v>
+      </c>
+    </row>
+    <row r="872" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A872" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B872" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C872" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D872" s="1">
+        <v>0</v>
+      </c>
+      <c r="E872" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F872" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G872" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="H872" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I872">
+        <v>822</v>
+      </c>
+      <c r="J872">
+        <v>0.62967994605280997</v>
+      </c>
+      <c r="K872">
+        <v>2.9362108217132099</v>
+      </c>
+    </row>
+    <row r="873" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A873" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B873" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C873" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D873" s="1">
+        <v>0</v>
+      </c>
+      <c r="E873" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F873" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G873" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H873" s="1">
+        <v>65461</v>
+      </c>
+      <c r="I873">
+        <v>668</v>
+      </c>
+      <c r="J873">
+        <v>0.642863713880933</v>
+      </c>
+      <c r="K873">
+        <v>3.2654385528034702</v>
+      </c>
+    </row>
+    <row r="874" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A874" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B874" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C874" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D874" s="1">
+        <v>0</v>
+      </c>
+      <c r="E874" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F874" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G874" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H874" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I874">
+        <v>827</v>
+      </c>
+      <c r="J874">
+        <v>0.65814881555778904</v>
+      </c>
+      <c r="K874">
+        <v>3.0215611509729698</v>
+      </c>
+    </row>
+    <row r="875" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A875" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B875" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C875" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D875" s="1">
+        <v>0</v>
+      </c>
+      <c r="E875" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F875" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G875" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H875" s="1">
+        <v>65028</v>
+      </c>
+      <c r="I875">
+        <v>697</v>
+      </c>
+      <c r="J875">
+        <v>0.65248503734781904</v>
+      </c>
+      <c r="K875">
+        <v>3.0723789699929598</v>
+      </c>
+    </row>
+    <row r="876" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A876" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B876" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C876" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D876" s="1">
+        <v>0</v>
+      </c>
+      <c r="E876" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F876" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G876" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H876" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I876">
+        <v>614</v>
+      </c>
+      <c r="J876">
+        <v>0.62561053162381497</v>
+      </c>
+      <c r="K876">
+        <v>3.1561177563059402</v>
+      </c>
+    </row>
+    <row r="877" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A877" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B877" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C877" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D877" s="1">
+        <v>0</v>
+      </c>
+      <c r="E877" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F877" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G877" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="H877" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I877">
+        <v>636</v>
+      </c>
+      <c r="J877">
+        <v>0.66744132686934499</v>
+      </c>
+      <c r="K877">
+        <v>3.5710040447207998</v>
+      </c>
+    </row>
+    <row r="878" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A878" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B878" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C878" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D878" s="1">
+        <v>0</v>
+      </c>
+      <c r="E878" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F878" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G878" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="H878" s="1">
+        <v>43004</v>
+      </c>
+      <c r="I878">
+        <v>508</v>
+      </c>
+      <c r="J878">
+        <v>0.65440732898520404</v>
+      </c>
+      <c r="K878">
+        <v>3.4060892802051099</v>
+      </c>
+    </row>
+    <row r="879" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A879" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B879" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C879" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D879" s="1">
+        <v>0</v>
+      </c>
+      <c r="E879" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F879" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G879" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="H879" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I879">
+        <v>808</v>
+      </c>
+      <c r="J879">
+        <v>0.64951634364328503</v>
+      </c>
+      <c r="K879">
+        <v>2.9678501511129798</v>
+      </c>
+    </row>
+    <row r="880" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A880" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B880" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C880" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D880" s="1">
+        <v>0</v>
+      </c>
+      <c r="E880" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F880" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G880" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H880" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I880">
+        <v>716</v>
+      </c>
+      <c r="J880">
+        <v>0.65959090088465699</v>
+      </c>
+      <c r="K880">
+        <v>3.13317037438012</v>
+      </c>
+    </row>
+    <row r="881" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A881" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B881" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C881" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D881" s="1">
+        <v>0</v>
+      </c>
+      <c r="E881" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F881" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G881" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="H881" s="1">
+        <v>62170</v>
+      </c>
+      <c r="I881">
+        <v>786</v>
+      </c>
+      <c r="J881">
+        <v>0.57135248154922702</v>
+      </c>
+      <c r="K881">
+        <v>2.8202650463938901</v>
+      </c>
+    </row>
+    <row r="882" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A882" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B882" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C882" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D882" s="1">
+        <v>0</v>
+      </c>
+      <c r="E882" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F882" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G882" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="H882" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I882">
+        <v>780</v>
+      </c>
+      <c r="J882">
+        <v>0.61361668561618798</v>
+      </c>
+      <c r="K882">
+        <v>2.8555010381792698</v>
+      </c>
+    </row>
+    <row r="883" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A883" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B883" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C883" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D883" s="1">
+        <v>0</v>
+      </c>
+      <c r="E883" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F883" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G883" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="H883" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I883">
+        <v>579</v>
+      </c>
+      <c r="J883">
+        <v>0.64848823836629599</v>
+      </c>
+      <c r="K883">
+        <v>2.8970046612083098</v>
+      </c>
+    </row>
+    <row r="884" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A884" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B884" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C884" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D884" s="1">
+        <v>0</v>
+      </c>
+      <c r="E884" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F884" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G884" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="H884" s="1">
+        <v>54168</v>
+      </c>
+      <c r="I884">
+        <v>479</v>
+      </c>
+      <c r="J884">
+        <v>0.651747993664753</v>
+      </c>
+      <c r="K884">
+        <v>2.8666618433841098</v>
+      </c>
+    </row>
+    <row r="885" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A885" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B885" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C885" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D885" s="1">
+        <v>0</v>
+      </c>
+      <c r="E885" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F885" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G885" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="H885" s="1">
+        <v>57605</v>
+      </c>
+      <c r="I885">
+        <v>603</v>
+      </c>
+      <c r="J885">
+        <v>0.66903127116931804</v>
+      </c>
+      <c r="K885">
+        <v>2.94348104944318</v>
+      </c>
+    </row>
+    <row r="886" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A886" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B886" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C886" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D886" s="1">
+        <v>0</v>
+      </c>
+      <c r="E886" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F886" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G886" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="H886" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I886">
+        <v>714</v>
+      </c>
+      <c r="J886">
+        <v>0.625757642348302</v>
+      </c>
+      <c r="K886">
+        <v>3.0028008043584098</v>
+      </c>
+    </row>
+    <row r="887" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A887" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B887" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C887" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D887" s="1">
+        <v>0</v>
+      </c>
+      <c r="E887" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F887" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G887" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="H887" s="1">
+        <v>64755</v>
+      </c>
+      <c r="I887">
+        <v>720</v>
+      </c>
+      <c r="J887">
+        <v>0.620409120853185</v>
+      </c>
+      <c r="K887">
+        <v>3.14831211777466</v>
+      </c>
+    </row>
+    <row r="888" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A888" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B888" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C888" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D888" s="1">
+        <v>0</v>
+      </c>
+      <c r="E888" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F888" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G888" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="H888" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I888">
+        <v>640</v>
+      </c>
+      <c r="J888">
+        <v>0.62858490043680304</v>
+      </c>
+      <c r="K888">
+        <v>3.81879854122566</v>
+      </c>
+    </row>
+    <row r="889" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A889" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B889" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C889" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D889" s="1">
+        <v>0</v>
+      </c>
+      <c r="E889" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F889" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G889" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="H889" s="1">
+        <v>62854</v>
+      </c>
+      <c r="I889">
+        <v>531</v>
+      </c>
+      <c r="J889">
+        <v>0.61251234422367795</v>
+      </c>
+      <c r="K889">
+        <v>3.5112811600373499</v>
+      </c>
+    </row>
+    <row r="890" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A890" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B890" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C890" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D890" s="1">
+        <v>0</v>
+      </c>
+      <c r="E890" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F890" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G890" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="H890" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I890">
+        <v>705</v>
+      </c>
+      <c r="J890">
+        <v>0.62007753013584599</v>
+      </c>
+      <c r="K890">
+        <v>3.0788359459188301</v>
+      </c>
+    </row>
+    <row r="891" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A891" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B891" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C891" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D891" s="1">
+        <v>0</v>
+      </c>
+      <c r="E891" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F891" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G891" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="H891" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I891">
+        <v>905</v>
+      </c>
+      <c r="J891">
+        <v>0.62376858594042495</v>
+      </c>
+      <c r="K891">
+        <v>2.60703478065202</v>
+      </c>
+    </row>
+    <row r="892" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A892" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B892" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C892" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D892" s="1">
+        <v>0</v>
+      </c>
+      <c r="E892" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F892" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G892" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="H892" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I892">
+        <v>951</v>
+      </c>
+      <c r="J892">
+        <v>0.64762263589777103</v>
+      </c>
+      <c r="K892">
+        <v>2.5057672391648</v>
+      </c>
+    </row>
+    <row r="893" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A893" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B893" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C893" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D893" s="1">
+        <v>0</v>
+      </c>
+      <c r="E893" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F893" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G893" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="H893" s="1">
+        <v>27076</v>
+      </c>
+      <c r="I893">
+        <v>157</v>
+      </c>
+      <c r="J893">
+        <v>0.65229700502065902</v>
+      </c>
+      <c r="K893">
+        <v>3.9444511282252201</v>
+      </c>
+    </row>
+    <row r="894" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A894" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B894" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C894" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D894" s="1">
+        <v>0</v>
+      </c>
+      <c r="E894" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F894" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G894" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="H894" s="1">
+        <v>66063</v>
+      </c>
+      <c r="I894">
+        <v>447</v>
+      </c>
+      <c r="J894">
+        <v>0.66492596419031802</v>
+      </c>
+      <c r="K894">
+        <v>3.67518834783223</v>
+      </c>
+    </row>
+    <row r="895" spans="1:11" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A895" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B895" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C895" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D895" s="1">
+        <v>0</v>
+      </c>
+      <c r="E895" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F895" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G895" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="H895" s="1">
+        <v>62412</v>
+      </c>
+      <c r="I895">
+        <v>651</v>
+      </c>
+      <c r="J895">
+        <v>0.63549398937018198</v>
+      </c>
+      <c r="K895">
+        <v>3.2530417391525401</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K781" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <autoFilter ref="A1:K895" xr:uid="{00000000-0001-0000-0500-000000000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="control"/>

</xml_diff>